<commit_message>
experiment 1 almost done
</commit_message>
<xml_diff>
--- a/Experiment1.xlsx
+++ b/Experiment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kubilayagi/Documents/UCLA/physics4al/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A05BCCF-1734-A84C-89B6-B42A93FC744C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B8E5AF-C27A-1146-B602-680FFF1ED64C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="1000" windowWidth="31360" windowHeight="16560" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1147,7 +1147,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1800" baseline="0"/>
-              <a:t> Track Velocity, </a:t>
+              <a:t> Track Acceleration, </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1800"/>
@@ -1696,7 +1696,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Velocity (m/s)</a:t>
+                  <a:t>Acceleration (m/s^2)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -13818,8 +13818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C4F159-5AE7-0147-BE59-DB5520426F9D}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="H34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
almost halfway done with exp2 report
</commit_message>
<xml_diff>
--- a/Experiment1.xlsx
+++ b/Experiment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kubilayagi/Documents/UCLA/physics4al/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B8E5AF-C27A-1146-B602-680FFF1ED64C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0128C3-6FA8-4241-8FDF-7B939D7E3906}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="1000" windowWidth="31360" windowHeight="16560" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="52">
   <si>
     <t>glider</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>mean acceleration</t>
+  </si>
+  <si>
+    <t>std dev</t>
   </si>
 </sst>
 </file>
@@ -13816,10 +13819,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C4F159-5AE7-0147-BE59-DB5520426F9D}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W46" sqref="W46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13834,12 +13837,12 @@
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -13868,7 +13871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2.6349999999999998</v>
       </c>
@@ -13902,8 +13905,11 @@
       <c r="K3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2.96</v>
       </c>
@@ -13938,8 +13944,16 @@
         <f>AVERAGE(I3:I38)</f>
         <v>9.7109156473998592E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f>STDEV(I3:I38)</f>
+        <v>2.3351826802475995E-2</v>
+      </c>
+      <c r="M4">
+        <f>COUNT(I3:I38)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>3.1659999999999999</v>
       </c>
@@ -13971,7 +13985,7 @@
         <v>8.7102123801916551E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3.3290000000000002</v>
       </c>
@@ -14003,7 +14017,7 @@
         <v>9.5533795080008518E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>3.4689999999999999</v>
       </c>
@@ -14035,7 +14049,7 @@
         <v>9.3332555562039232E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>3.5939999999999999</v>
       </c>
@@ -14067,7 +14081,7 @@
         <v>9.1660746061437606E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>3.706</v>
       </c>
@@ -14099,7 +14113,7 @@
         <v>9.7288640428669512E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>3.8109999999999999</v>
       </c>
@@ -14131,7 +14145,7 @@
         <v>9.1418625082157062E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>3.9079999999999999</v>
       </c>
@@ -14163,7 +14177,7 @@
         <v>9.6443726871372593E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>4</v>
       </c>
@@ -14195,7 +14209,7 @@
         <v>0.10016778103321571</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>4.0869999999999997</v>
       </c>
@@ -14227,7 +14241,7 @@
         <v>8.5813338825419846E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>4.17</v>
       </c>
@@ -14259,7 +14273,7 @@
         <v>9.737098344690398E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>4.2489999999999997</v>
       </c>
@@ -14291,7 +14305,7 @@
         <v>0.10822510822511691</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>4.3259999999999996</v>
       </c>

</xml_diff>